<commit_message>
Add survey name on importing new survey responses
</commit_message>
<xml_diff>
--- a/packages/meditrak-server/src/tests/testData/surveyResponses/valid.xlsx
+++ b/packages/meditrak-server/src/tests/testData/surveyResponses/valid.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Edwin/Documents/Git/meditrak-server/src/tests/testData/surveyResponses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Edwin/Documents/Git/tupaia/packages/meditrak-server/src/tests/testData/surveyResponses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF844F8-3105-0647-A350-F7315F81E7DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BEE6EE-C435-A342-9557-F890D419385B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Basic Clinic Data..." sheetId="1" r:id="rId1"/>
+    <sheet name="Test Survey" sheetId="1" r:id="rId1"/>
     <sheet name="Facility Fundamen..." sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateCount="1" iterateDelta="1E-4"/>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Allow importing new responses without an initial response (#1543)
</commit_message>
<xml_diff>
--- a/packages/meditrak-server/src/tests/testData/surveyResponses/valid.xlsx
+++ b/packages/meditrak-server/src/tests/testData/surveyResponses/valid.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Edwin/Documents/Git/meditrak-server/src/tests/testData/surveyResponses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Edwin/Documents/Git/tupaia/packages/meditrak-server/src/tests/testData/surveyResponses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF844F8-3105-0647-A350-F7315F81E7DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BEE6EE-C435-A342-9557-F890D419385B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Basic Clinic Data..." sheetId="1" r:id="rId1"/>
+    <sheet name="Test Survey" sheetId="1" r:id="rId1"/>
     <sheet name="Facility Fundamen..." sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateCount="1" iterateDelta="1E-4"/>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>